<commit_message>
Updated Examples for Chapter 2
</commit_message>
<xml_diff>
--- a/AMPL_Book_Examples.xlsx
+++ b/AMPL_Book_Examples.xlsx
@@ -4,202 +4,298 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="20115" windowHeight="12090" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="20115" windowHeight="12090" tabRatio="703" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="diet0" sheetId="4" r:id="rId1"/>
     <sheet name="diet2" sheetId="5" r:id="rId2"/>
     <sheet name="diet2a" sheetId="6" r:id="rId3"/>
     <sheet name="diet2b" sheetId="7" r:id="rId4"/>
+    <sheet name="diet2aForceInt" sheetId="8" r:id="rId5"/>
+    <sheet name="diet2aIntRestrict" sheetId="9" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="amt" localSheetId="0">diet0!$B$24:$E$31</definedName>
     <definedName name="amt" localSheetId="1">diet2!$B$25:$G$32</definedName>
     <definedName name="amt" localSheetId="2">diet2a!$B$25:$G$32</definedName>
+    <definedName name="amt" localSheetId="4">diet2aForceInt!$B$25:$G$32</definedName>
+    <definedName name="amt" localSheetId="5">diet2aIntRestrict!$B$25:$G$32</definedName>
     <definedName name="amt" localSheetId="3">diet2b!$B$25:$G$32</definedName>
     <definedName name="amt.badindex" localSheetId="0" hidden="1">1</definedName>
     <definedName name="amt.badindex" localSheetId="1" hidden="1">1</definedName>
     <definedName name="amt.badindex" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="amt.badindex" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="amt.badindex" localSheetId="5" hidden="1">1</definedName>
     <definedName name="amt.badindex" localSheetId="3" hidden="1">1</definedName>
     <definedName name="amt.columnindex" localSheetId="0" hidden="1">diet0!$B$23:$E$23</definedName>
     <definedName name="amt.columnindex" localSheetId="1" hidden="1">diet2!$B$24:$G$24</definedName>
     <definedName name="amt.columnindex" localSheetId="2" hidden="1">diet2a!$B$24:$G$24</definedName>
+    <definedName name="amt.columnindex" localSheetId="4" hidden="1">diet2aForceInt!$B$24:$G$24</definedName>
+    <definedName name="amt.columnindex" localSheetId="5" hidden="1">diet2aIntRestrict!$B$24:$G$24</definedName>
     <definedName name="amt.columnindex" localSheetId="3" hidden="1">diet2b!$B$24:$G$24</definedName>
     <definedName name="amt.columnindex.dirn" localSheetId="0" hidden="1">"column"</definedName>
     <definedName name="amt.columnindex.dirn" localSheetId="1" hidden="1">"column"</definedName>
     <definedName name="amt.columnindex.dirn" localSheetId="2" hidden="1">"column"</definedName>
+    <definedName name="amt.columnindex.dirn" localSheetId="4" hidden="1">"column"</definedName>
+    <definedName name="amt.columnindex.dirn" localSheetId="5" hidden="1">"column"</definedName>
     <definedName name="amt.columnindex.dirn" localSheetId="3" hidden="1">"column"</definedName>
     <definedName name="amt.firstindex" localSheetId="0" hidden="1">"column"</definedName>
     <definedName name="amt.firstindex" localSheetId="1" hidden="1">"column"</definedName>
     <definedName name="amt.firstindex" localSheetId="2" hidden="1">"column"</definedName>
+    <definedName name="amt.firstindex" localSheetId="4" hidden="1">"column"</definedName>
+    <definedName name="amt.firstindex" localSheetId="5" hidden="1">"column"</definedName>
     <definedName name="amt.firstindex" localSheetId="3" hidden="1">"column"</definedName>
     <definedName name="amt.rowindex" localSheetId="0" hidden="1">diet0!$A$24:$A$31</definedName>
     <definedName name="amt.rowindex" localSheetId="1" hidden="1">diet2!$A$25:$A$32</definedName>
     <definedName name="amt.rowindex" localSheetId="2" hidden="1">diet2a!$A$25:$A$32</definedName>
+    <definedName name="amt.rowindex" localSheetId="4" hidden="1">diet2aForceInt!$A$25:$A$32</definedName>
+    <definedName name="amt.rowindex" localSheetId="5" hidden="1">diet2aIntRestrict!$A$25:$A$32</definedName>
     <definedName name="amt.rowindex" localSheetId="3" hidden="1">diet2b!$A$25:$A$32</definedName>
     <definedName name="amt.rowindex.dirn" localSheetId="0" hidden="1">"row"</definedName>
     <definedName name="amt.rowindex.dirn" localSheetId="1" hidden="1">"row"</definedName>
     <definedName name="amt.rowindex.dirn" localSheetId="2" hidden="1">"row"</definedName>
+    <definedName name="amt.rowindex.dirn" localSheetId="4" hidden="1">"row"</definedName>
+    <definedName name="amt.rowindex.dirn" localSheetId="5" hidden="1">"row"</definedName>
     <definedName name="amt.rowindex.dirn" localSheetId="3" hidden="1">"row"</definedName>
     <definedName name="amtcolumnindex.dirn" localSheetId="0">"Column"</definedName>
     <definedName name="amtcolumnindex.dirn" localSheetId="1">"Column"</definedName>
     <definedName name="amtcolumnindex.dirn" localSheetId="2">"Column"</definedName>
+    <definedName name="amtcolumnindex.dirn" localSheetId="4">"Column"</definedName>
+    <definedName name="amtcolumnindex.dirn" localSheetId="5">"Column"</definedName>
     <definedName name="amtcolumnindex.dirn" localSheetId="3">"Column"</definedName>
     <definedName name="amtrowindex.dirn" localSheetId="0">"Row"</definedName>
     <definedName name="amtrowindex.dirn" localSheetId="1">"Row"</definedName>
     <definedName name="amtrowindex.dirn" localSheetId="2">"Row"</definedName>
+    <definedName name="amtrowindex.dirn" localSheetId="4">"Row"</definedName>
+    <definedName name="amtrowindex.dirn" localSheetId="5">"Row"</definedName>
     <definedName name="amtrowindex.dirn" localSheetId="3">"Row"</definedName>
     <definedName name="Buy" localSheetId="0">diet0!$F$4:$F$11</definedName>
     <definedName name="Buy" localSheetId="1">diet2!$F$4:$F$11</definedName>
     <definedName name="Buy" localSheetId="2">diet2a!$F$4:$F$11</definedName>
+    <definedName name="Buy" localSheetId="4">diet2aForceInt!$F$4:$F$11</definedName>
+    <definedName name="Buy" localSheetId="5">diet2aIntRestrict!$F$4:$F$11</definedName>
     <definedName name="Buy" localSheetId="3">diet2b!$F$4:$F$11</definedName>
     <definedName name="Buy.badindex" localSheetId="0" hidden="1">1</definedName>
     <definedName name="Buy.badindex" localSheetId="1" hidden="1">1</definedName>
     <definedName name="Buy.badindex" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="Buy.badindex" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="Buy.badindex" localSheetId="5" hidden="1">1</definedName>
     <definedName name="Buy.badindex" localSheetId="3" hidden="1">1</definedName>
     <definedName name="Buy.rowindex" localSheetId="0" hidden="1">diet0!$A$4:$A$11</definedName>
     <definedName name="Buy.rowindex" localSheetId="1" hidden="1">diet2!$A$4:$A$11</definedName>
     <definedName name="Buy.rowindex" localSheetId="2" hidden="1">diet2a!$A$4:$A$11</definedName>
+    <definedName name="Buy.rowindex" localSheetId="4" hidden="1">diet2aForceInt!$A$4:$A$11</definedName>
+    <definedName name="Buy.rowindex" localSheetId="5" hidden="1">diet2aIntRestrict!$A$4:$A$11</definedName>
     <definedName name="Buy.rowindex" localSheetId="3" hidden="1">diet2b!$A$4:$A$11</definedName>
     <definedName name="Buy.rowindex.dirn" localSheetId="0" hidden="1">"row"</definedName>
     <definedName name="Buy.rowindex.dirn" localSheetId="1" hidden="1">"row"</definedName>
     <definedName name="Buy.rowindex.dirn" localSheetId="2" hidden="1">"row"</definedName>
+    <definedName name="Buy.rowindex.dirn" localSheetId="4" hidden="1">"row"</definedName>
+    <definedName name="Buy.rowindex.dirn" localSheetId="5" hidden="1">"row"</definedName>
     <definedName name="Buy.rowindex.dirn" localSheetId="3" hidden="1">"row"</definedName>
     <definedName name="cost" localSheetId="0">diet0!$B$4:$B$11</definedName>
     <definedName name="cost" localSheetId="1">diet2!$B$4:$B$11</definedName>
     <definedName name="cost" localSheetId="2">diet2a!$B$4:$B$11</definedName>
+    <definedName name="cost" localSheetId="4">diet2aForceInt!$B$4:$B$11</definedName>
+    <definedName name="cost" localSheetId="5">diet2aIntRestrict!$B$4:$B$11</definedName>
     <definedName name="cost" localSheetId="3">diet2b!$B$4:$B$11</definedName>
     <definedName name="cost.badindex" localSheetId="0" hidden="1">1</definedName>
     <definedName name="cost.badindex" localSheetId="1" hidden="1">1</definedName>
     <definedName name="cost.badindex" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="cost.badindex" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="cost.badindex" localSheetId="5" hidden="1">1</definedName>
     <definedName name="cost.badindex" localSheetId="3" hidden="1">1</definedName>
     <definedName name="cost.rowindex" localSheetId="0" hidden="1">diet0!$A$4:$A$11</definedName>
     <definedName name="cost.rowindex" localSheetId="1" hidden="1">diet2!$A$4:$A$11</definedName>
     <definedName name="cost.rowindex" localSheetId="2" hidden="1">diet2a!$A$4:$A$11</definedName>
+    <definedName name="cost.rowindex" localSheetId="4" hidden="1">diet2aForceInt!$A$4:$A$11</definedName>
+    <definedName name="cost.rowindex" localSheetId="5" hidden="1">diet2aIntRestrict!$A$4:$A$11</definedName>
     <definedName name="cost.rowindex" localSheetId="3" hidden="1">diet2b!$A$4:$A$11</definedName>
     <definedName name="cost.rowindex.dirn" localSheetId="0" hidden="1">"row"</definedName>
     <definedName name="cost.rowindex.dirn" localSheetId="1" hidden="1">"row"</definedName>
     <definedName name="cost.rowindex.dirn" localSheetId="2" hidden="1">"row"</definedName>
+    <definedName name="cost.rowindex.dirn" localSheetId="4" hidden="1">"row"</definedName>
+    <definedName name="cost.rowindex.dirn" localSheetId="5" hidden="1">"row"</definedName>
     <definedName name="cost.rowindex.dirn" localSheetId="3" hidden="1">"row"</definedName>
     <definedName name="costcolumnindex.dirn" localSheetId="0">"Column"</definedName>
     <definedName name="costcolumnindex.dirn" localSheetId="1">"Column"</definedName>
     <definedName name="costcolumnindex.dirn" localSheetId="2">"Column"</definedName>
+    <definedName name="costcolumnindex.dirn" localSheetId="4">"Column"</definedName>
+    <definedName name="costcolumnindex.dirn" localSheetId="5">"Column"</definedName>
     <definedName name="costcolumnindex.dirn" localSheetId="3">"Column"</definedName>
     <definedName name="costrowindex.dirn" localSheetId="0">"Row"</definedName>
     <definedName name="costrowindex.dirn" localSheetId="1">"Row"</definedName>
     <definedName name="costrowindex.dirn" localSheetId="2">"Row"</definedName>
+    <definedName name="costrowindex.dirn" localSheetId="4">"Row"</definedName>
+    <definedName name="costrowindex.dirn" localSheetId="5">"Row"</definedName>
     <definedName name="costrowindex.dirn" localSheetId="3">"Row"</definedName>
     <definedName name="Diet" localSheetId="0">diet0!$F$15:$F$18</definedName>
     <definedName name="Diet" localSheetId="1">diet2!$F$16:$F$21</definedName>
     <definedName name="Diet" localSheetId="2">diet2a!$F$16:$F$21</definedName>
+    <definedName name="Diet" localSheetId="4">diet2aForceInt!$F$16:$F$21</definedName>
+    <definedName name="Diet" localSheetId="5">diet2aIntRestrict!$F$16:$F$21</definedName>
     <definedName name="Diet" localSheetId="3">diet2b!$F$16:$F$21</definedName>
     <definedName name="Diet.badindex" localSheetId="0" hidden="1">1</definedName>
     <definedName name="Diet.badindex" localSheetId="1" hidden="1">1</definedName>
     <definedName name="Diet.badindex" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="Diet.badindex" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="Diet.badindex" localSheetId="5" hidden="1">1</definedName>
     <definedName name="Diet.badindex" localSheetId="3" hidden="1">1</definedName>
     <definedName name="Diet.rowindex" localSheetId="0" hidden="1">diet0!$A$15:$A$18</definedName>
     <definedName name="Diet.rowindex" localSheetId="1" hidden="1">diet2!$A$16:$A$21</definedName>
     <definedName name="Diet.rowindex" localSheetId="2" hidden="1">diet2a!$A$16:$A$21</definedName>
+    <definedName name="Diet.rowindex" localSheetId="4" hidden="1">diet2aForceInt!$A$16:$A$21</definedName>
+    <definedName name="Diet.rowindex" localSheetId="5" hidden="1">diet2aIntRestrict!$A$16:$A$21</definedName>
     <definedName name="Diet.rowindex" localSheetId="3" hidden="1">diet2b!$A$16:$A$21</definedName>
     <definedName name="Diet.rowindex.dirn" localSheetId="0" hidden="1">"row"</definedName>
     <definedName name="Diet.rowindex.dirn" localSheetId="1" hidden="1">"row"</definedName>
     <definedName name="Diet.rowindex.dirn" localSheetId="2" hidden="1">"row"</definedName>
+    <definedName name="Diet.rowindex.dirn" localSheetId="4" hidden="1">"row"</definedName>
+    <definedName name="Diet.rowindex.dirn" localSheetId="5" hidden="1">"row"</definedName>
     <definedName name="Diet.rowindex.dirn" localSheetId="3" hidden="1">"row"</definedName>
     <definedName name="f_max" localSheetId="0">diet0!$D$4:$D$11</definedName>
     <definedName name="f_max" localSheetId="1">diet2!$D$4:$D$11</definedName>
     <definedName name="f_max" localSheetId="2">diet2a!$D$4:$D$11</definedName>
+    <definedName name="f_max" localSheetId="4">diet2aForceInt!$D$4:$D$11</definedName>
+    <definedName name="f_max" localSheetId="5">diet2aIntRestrict!$D$4:$D$11</definedName>
     <definedName name="f_max" localSheetId="3">diet2b!$D$4:$D$11</definedName>
     <definedName name="f_max.badindex" localSheetId="0" hidden="1">1</definedName>
     <definedName name="f_max.badindex" localSheetId="1" hidden="1">1</definedName>
     <definedName name="f_max.badindex" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="f_max.badindex" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="f_max.badindex" localSheetId="5" hidden="1">1</definedName>
     <definedName name="f_max.badindex" localSheetId="3" hidden="1">1</definedName>
     <definedName name="f_max.rowindex" localSheetId="0" hidden="1">diet0!$A$4:$A$11</definedName>
     <definedName name="f_max.rowindex" localSheetId="1" hidden="1">diet2!$A$4:$A$11</definedName>
     <definedName name="f_max.rowindex" localSheetId="2" hidden="1">diet2a!$A$4:$A$11</definedName>
+    <definedName name="f_max.rowindex" localSheetId="4" hidden="1">diet2aForceInt!$A$4:$A$11</definedName>
+    <definedName name="f_max.rowindex" localSheetId="5" hidden="1">diet2aIntRestrict!$A$4:$A$11</definedName>
     <definedName name="f_max.rowindex" localSheetId="3" hidden="1">diet2b!$A$4:$A$11</definedName>
     <definedName name="f_max.rowindex.dirn" localSheetId="0" hidden="1">"row"</definedName>
     <definedName name="f_max.rowindex.dirn" localSheetId="1" hidden="1">"row"</definedName>
     <definedName name="f_max.rowindex.dirn" localSheetId="2" hidden="1">"row"</definedName>
+    <definedName name="f_max.rowindex.dirn" localSheetId="4" hidden="1">"row"</definedName>
+    <definedName name="f_max.rowindex.dirn" localSheetId="5" hidden="1">"row"</definedName>
     <definedName name="f_max.rowindex.dirn" localSheetId="3" hidden="1">"row"</definedName>
     <definedName name="f_min" localSheetId="0">diet0!$C$4:$C$11</definedName>
     <definedName name="f_min" localSheetId="1">diet2!$C$4:$C$11</definedName>
     <definedName name="f_min" localSheetId="2">diet2a!$C$4:$C$11</definedName>
+    <definedName name="f_min" localSheetId="4">diet2aForceInt!$C$4:$C$11</definedName>
+    <definedName name="f_min" localSheetId="5">diet2aIntRestrict!$C$4:$C$11</definedName>
     <definedName name="f_min" localSheetId="3">diet2b!$C$4:$C$11</definedName>
     <definedName name="f_min.badindex" localSheetId="0" hidden="1">1</definedName>
     <definedName name="f_min.badindex" localSheetId="1" hidden="1">1</definedName>
     <definedName name="f_min.badindex" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="f_min.badindex" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="f_min.badindex" localSheetId="5" hidden="1">1</definedName>
     <definedName name="f_min.badindex" localSheetId="3" hidden="1">1</definedName>
     <definedName name="f_min.rowindex" localSheetId="0" hidden="1">diet0!$A$4:$A$11</definedName>
     <definedName name="f_min.rowindex" localSheetId="1" hidden="1">diet2!$A$4:$A$11</definedName>
     <definedName name="f_min.rowindex" localSheetId="2" hidden="1">diet2a!$A$4:$A$11</definedName>
+    <definedName name="f_min.rowindex" localSheetId="4" hidden="1">diet2aForceInt!$A$4:$A$11</definedName>
+    <definedName name="f_min.rowindex" localSheetId="5" hidden="1">diet2aIntRestrict!$A$4:$A$11</definedName>
     <definedName name="f_min.rowindex" localSheetId="3" hidden="1">diet2b!$A$4:$A$11</definedName>
     <definedName name="f_min.rowindex.dirn" localSheetId="0" hidden="1">"row"</definedName>
     <definedName name="f_min.rowindex.dirn" localSheetId="1" hidden="1">"row"</definedName>
     <definedName name="f_min.rowindex.dirn" localSheetId="2" hidden="1">"row"</definedName>
+    <definedName name="f_min.rowindex.dirn" localSheetId="4" hidden="1">"row"</definedName>
+    <definedName name="f_min.rowindex.dirn" localSheetId="5" hidden="1">"row"</definedName>
     <definedName name="f_min.rowindex.dirn" localSheetId="3" hidden="1">"row"</definedName>
     <definedName name="FOOD" localSheetId="0">diet0!$A$4:$A$11</definedName>
     <definedName name="FOOD" localSheetId="1">diet2!$A$4:$A$11</definedName>
     <definedName name="FOOD" localSheetId="2">diet2a!$A$4:$A$11</definedName>
+    <definedName name="FOOD" localSheetId="4">diet2aForceInt!$A$4:$A$11</definedName>
+    <definedName name="FOOD" localSheetId="5">diet2aIntRestrict!$A$4:$A$11</definedName>
     <definedName name="FOOD" localSheetId="3">diet2b!$A$4:$A$11</definedName>
     <definedName name="FOOD.dirn" localSheetId="0" hidden="1">"row"</definedName>
     <definedName name="FOOD.dirn" localSheetId="1" hidden="1">"row"</definedName>
     <definedName name="FOOD.dirn" localSheetId="2" hidden="1">"row"</definedName>
+    <definedName name="FOOD.dirn" localSheetId="4" hidden="1">"row"</definedName>
+    <definedName name="FOOD.dirn" localSheetId="5" hidden="1">"row"</definedName>
     <definedName name="FOOD.dirn" localSheetId="3" hidden="1">"row"</definedName>
     <definedName name="n_max" localSheetId="0">diet0!$C$15:$C$18</definedName>
     <definedName name="n_max" localSheetId="1">diet2!$C$16:$C$21</definedName>
     <definedName name="n_max" localSheetId="2">diet2a!$C$16:$C$21</definedName>
+    <definedName name="n_max" localSheetId="4">diet2aForceInt!$C$16:$C$21</definedName>
+    <definedName name="n_max" localSheetId="5">diet2aIntRestrict!$C$16:$C$21</definedName>
     <definedName name="n_max" localSheetId="3">diet2b!$C$16:$C$21</definedName>
     <definedName name="n_max.badindex" localSheetId="0" hidden="1">1</definedName>
     <definedName name="n_max.badindex" localSheetId="1" hidden="1">1</definedName>
     <definedName name="n_max.badindex" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="n_max.badindex" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="n_max.badindex" localSheetId="5" hidden="1">1</definedName>
     <definedName name="n_max.badindex" localSheetId="3" hidden="1">1</definedName>
     <definedName name="n_max.rowindex" localSheetId="0" hidden="1">diet0!$A$15:$A$18</definedName>
     <definedName name="n_max.rowindex" localSheetId="1" hidden="1">diet2!$A$16:$A$21</definedName>
     <definedName name="n_max.rowindex" localSheetId="2" hidden="1">diet2a!$A$16:$A$21</definedName>
+    <definedName name="n_max.rowindex" localSheetId="4" hidden="1">diet2aForceInt!$A$16:$A$21</definedName>
+    <definedName name="n_max.rowindex" localSheetId="5" hidden="1">diet2aIntRestrict!$A$16:$A$21</definedName>
     <definedName name="n_max.rowindex" localSheetId="3" hidden="1">diet2b!$A$16:$A$21</definedName>
     <definedName name="n_max.rowindex.dirn" localSheetId="0" hidden="1">"row"</definedName>
     <definedName name="n_max.rowindex.dirn" localSheetId="1" hidden="1">"row"</definedName>
     <definedName name="n_max.rowindex.dirn" localSheetId="2" hidden="1">"row"</definedName>
+    <definedName name="n_max.rowindex.dirn" localSheetId="4" hidden="1">"row"</definedName>
+    <definedName name="n_max.rowindex.dirn" localSheetId="5" hidden="1">"row"</definedName>
     <definedName name="n_max.rowindex.dirn" localSheetId="3" hidden="1">"row"</definedName>
     <definedName name="n_min" localSheetId="0">diet0!$B$15:$B$18</definedName>
     <definedName name="n_min" localSheetId="1">diet2!$B$16:$B$21</definedName>
     <definedName name="n_min" localSheetId="2">diet2a!$B$16:$B$21</definedName>
+    <definedName name="n_min" localSheetId="4">diet2aForceInt!$B$16:$B$21</definedName>
+    <definedName name="n_min" localSheetId="5">diet2aIntRestrict!$B$16:$B$21</definedName>
     <definedName name="n_min" localSheetId="3">diet2b!$B$16:$B$21</definedName>
     <definedName name="n_min.badindex" localSheetId="0" hidden="1">1</definedName>
     <definedName name="n_min.badindex" localSheetId="1" hidden="1">1</definedName>
     <definedName name="n_min.badindex" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="n_min.badindex" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="n_min.badindex" localSheetId="5" hidden="1">1</definedName>
     <definedName name="n_min.badindex" localSheetId="3" hidden="1">1</definedName>
     <definedName name="n_min.rowindex" localSheetId="0" hidden="1">diet0!$A$15:$A$18</definedName>
     <definedName name="n_min.rowindex" localSheetId="1" hidden="1">diet2!$A$16:$A$21</definedName>
     <definedName name="n_min.rowindex" localSheetId="2" hidden="1">diet2a!$A$16:$A$21</definedName>
+    <definedName name="n_min.rowindex" localSheetId="4" hidden="1">diet2aForceInt!$A$16:$A$21</definedName>
+    <definedName name="n_min.rowindex" localSheetId="5" hidden="1">diet2aIntRestrict!$A$16:$A$21</definedName>
     <definedName name="n_min.rowindex" localSheetId="3" hidden="1">diet2b!$A$16:$A$21</definedName>
     <definedName name="n_min.rowindex.dirn" localSheetId="0" hidden="1">"row"</definedName>
     <definedName name="n_min.rowindex.dirn" localSheetId="1" hidden="1">"row"</definedName>
     <definedName name="n_min.rowindex.dirn" localSheetId="2" hidden="1">"row"</definedName>
+    <definedName name="n_min.rowindex.dirn" localSheetId="4" hidden="1">"row"</definedName>
+    <definedName name="n_min.rowindex.dirn" localSheetId="5" hidden="1">"row"</definedName>
     <definedName name="n_min.rowindex.dirn" localSheetId="3" hidden="1">"row"</definedName>
     <definedName name="n_mincolumnindex.dirn" localSheetId="0">"Column"</definedName>
     <definedName name="n_mincolumnindex.dirn" localSheetId="1">"Column"</definedName>
     <definedName name="n_mincolumnindex.dirn" localSheetId="2">"Column"</definedName>
+    <definedName name="n_mincolumnindex.dirn" localSheetId="4">"Column"</definedName>
+    <definedName name="n_mincolumnindex.dirn" localSheetId="5">"Column"</definedName>
     <definedName name="n_mincolumnindex.dirn" localSheetId="3">"Column"</definedName>
     <definedName name="n_minrowindex.dirn" localSheetId="0">"Row"</definedName>
     <definedName name="n_minrowindex.dirn" localSheetId="1">"Row"</definedName>
     <definedName name="n_minrowindex.dirn" localSheetId="2">"Row"</definedName>
+    <definedName name="n_minrowindex.dirn" localSheetId="4">"Row"</definedName>
+    <definedName name="n_minrowindex.dirn" localSheetId="5">"Row"</definedName>
     <definedName name="n_minrowindex.dirn" localSheetId="3">"Row"</definedName>
     <definedName name="NUTR" localSheetId="0">diet0!$A$15:$A$18</definedName>
     <definedName name="NUTR" localSheetId="1">diet2!$A$16:$A$21</definedName>
     <definedName name="NUTR" localSheetId="2">diet2a!$A$16:$A$21</definedName>
+    <definedName name="NUTR" localSheetId="4">diet2aForceInt!$A$16:$A$21</definedName>
+    <definedName name="NUTR" localSheetId="5">diet2aIntRestrict!$A$16:$A$21</definedName>
     <definedName name="NUTR" localSheetId="3">diet2b!$A$16:$A$21</definedName>
     <definedName name="NUTR.dirn" localSheetId="0" hidden="1">"row"</definedName>
     <definedName name="NUTR.dirn" localSheetId="1" hidden="1">"row"</definedName>
     <definedName name="NUTR.dirn" localSheetId="2" hidden="1">"row"</definedName>
+    <definedName name="NUTR.dirn" localSheetId="4" hidden="1">"row"</definedName>
+    <definedName name="NUTR.dirn" localSheetId="5" hidden="1">"row"</definedName>
     <definedName name="NUTR.dirn" localSheetId="3" hidden="1">"row"</definedName>
     <definedName name="solve_result" localSheetId="0">diet0!$A$34</definedName>
     <definedName name="solve_result" localSheetId="1">diet2!$A$35</definedName>
     <definedName name="solve_result" localSheetId="2">diet2a!$A$35</definedName>
+    <definedName name="solve_result" localSheetId="4">diet2aForceInt!$A$35</definedName>
+    <definedName name="solve_result" localSheetId="5">diet2aIntRestrict!$A$35</definedName>
     <definedName name="solve_result" localSheetId="3">diet2b!$A$35</definedName>
     <definedName name="Total_Cost" localSheetId="0">diet0!$G$12</definedName>
     <definedName name="Total_Cost" localSheetId="1">diet2!$G$12</definedName>
     <definedName name="Total_Cost" localSheetId="2">diet2a!$G$12</definedName>
+    <definedName name="Total_Cost" localSheetId="4">diet2aForceInt!$G$12</definedName>
+    <definedName name="Total_Cost" localSheetId="5">diet2aIntRestrict!$G$12</definedName>
     <definedName name="Total_Cost" localSheetId="3">diet2b!$G$12</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -207,7 +303,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="32">
   <si>
     <t>TUR</t>
   </si>
@@ -404,7 +500,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -437,7 +533,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -450,6 +545,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -724,6 +822,456 @@
         <a:xfrm flipH="1" flipV="1">
           <a:off x="1819275" y="3790951"/>
           <a:ext cx="352425" cy="2524124"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="15875">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:prstDash val="dash"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>28574</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1247774" y="6315075"/>
+          <a:ext cx="3733801" cy="971550"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:prstDash val="dash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" i="1"/>
+            <a:t>round BEEF from 5.36061 to 6 and Spaghetti from 9.30605 to 10 to see that Sodium is  violated &gt;50K,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" i="1" baseline="0"/>
+            <a:t> (so now infeasible).</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" i="1"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" i="1"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" i="1"/>
+            <a:t>Note: "solved" here refers to the solution before</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" i="1" baseline="0"/>
+            <a:t> the "let" comands change the result.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" i="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Arrow Connector 2"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1809750" y="1857375"/>
+          <a:ext cx="1581150" cy="4467225"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="15875">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:prstDash val="dash"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>114303</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Arrow Connector 4"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1838325" y="685803"/>
+          <a:ext cx="1581150" cy="5619747"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="15875">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:prstDash val="dash"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="Freeform 12"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3457575" y="3752850"/>
+          <a:ext cx="495300" cy="2790825"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 476250 w 1304925"/>
+            <a:gd name="connsiteY0" fmla="*/ 2447925 h 2447925"/>
+            <a:gd name="connsiteX1" fmla="*/ 1304925 w 1304925"/>
+            <a:gd name="connsiteY1" fmla="*/ 485775 h 2447925"/>
+            <a:gd name="connsiteX2" fmla="*/ 0 w 1304925"/>
+            <a:gd name="connsiteY2" fmla="*/ 0 h 2447925"/>
+            <a:gd name="connsiteX0" fmla="*/ 0 w 1600200"/>
+            <a:gd name="connsiteY0" fmla="*/ 2790825 h 2790825"/>
+            <a:gd name="connsiteX1" fmla="*/ 1600200 w 1600200"/>
+            <a:gd name="connsiteY1" fmla="*/ 485775 h 2790825"/>
+            <a:gd name="connsiteX2" fmla="*/ 295275 w 1600200"/>
+            <a:gd name="connsiteY2" fmla="*/ 0 h 2790825"/>
+            <a:gd name="connsiteX0" fmla="*/ 0 w 371475"/>
+            <a:gd name="connsiteY0" fmla="*/ 2790825 h 2790825"/>
+            <a:gd name="connsiteX1" fmla="*/ 371475 w 371475"/>
+            <a:gd name="connsiteY1" fmla="*/ 2276475 h 2790825"/>
+            <a:gd name="connsiteX2" fmla="*/ 295275 w 371475"/>
+            <a:gd name="connsiteY2" fmla="*/ 0 h 2790825"/>
+            <a:gd name="connsiteX0" fmla="*/ 0 w 371475"/>
+            <a:gd name="connsiteY0" fmla="*/ 2790825 h 2790825"/>
+            <a:gd name="connsiteX1" fmla="*/ 371475 w 371475"/>
+            <a:gd name="connsiteY1" fmla="*/ 2276475 h 2790825"/>
+            <a:gd name="connsiteX2" fmla="*/ 238125 w 371475"/>
+            <a:gd name="connsiteY2" fmla="*/ 0 h 2790825"/>
+            <a:gd name="connsiteX0" fmla="*/ 0 w 495300"/>
+            <a:gd name="connsiteY0" fmla="*/ 2790825 h 2790825"/>
+            <a:gd name="connsiteX1" fmla="*/ 495300 w 495300"/>
+            <a:gd name="connsiteY1" fmla="*/ 2257425 h 2790825"/>
+            <a:gd name="connsiteX2" fmla="*/ 238125 w 495300"/>
+            <a:gd name="connsiteY2" fmla="*/ 0 h 2790825"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="495300" h="2790825">
+              <a:moveTo>
+                <a:pt x="0" y="2790825"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="495300" y="2257425"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="238125" y="0"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:prstDash val="dash"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>57149</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>142876</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1276349" y="6238876"/>
+          <a:ext cx="3638551" cy="1190624"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:prstDash val="dash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" i="1"/>
+            <a:t>ADDED AMPL</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" i="1" baseline="0"/>
+            <a:t> integrality restriction into "</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" i="1" baseline="0"/>
+            <a:t>var Buy</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" i="1" baseline="0"/>
+            <a:t>"  and removed two previous "let" commands, so solver forces integer result and gets a feasible result.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" i="1" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" i="1" baseline="0"/>
+            <a:t>Note: Switched solver back to "cbc" because "IPOPT" wouldn't provide an integer result.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" i="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Arrow Connector 3"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4219575" y="1476375"/>
+          <a:ext cx="1000125" cy="4762500"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1489,10 +2037,10 @@
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="20" t="s">
+      <c r="A34" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="B34" s="20"/>
+      <c r="B34" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1731,7 +2279,7 @@
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="22" t="s">
+      <c r="F14" s="21" t="s">
         <v>31</v>
       </c>
       <c r="G14" s="5"/>
@@ -1746,7 +2294,7 @@
       <c r="C15" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F15" s="21" t="s">
+      <c r="F15" s="20" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2048,10 +2596,10 @@
       </c>
     </row>
     <row r="35" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="19" t="s">
+      <c r="A35" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="B35" s="19"/>
+      <c r="B35" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2283,15 +2831,15 @@
       <c r="G13" s="5"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="24" t="s">
+      <c r="C14" s="23" t="s">
         <v>30</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="23" t="s">
+      <c r="F14" s="22" t="s">
         <v>31</v>
       </c>
       <c r="G14" s="5"/>
@@ -2306,7 +2854,7 @@
       <c r="C15" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F15" s="21" t="s">
+      <c r="F15" s="20" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2608,10 +3156,10 @@
       </c>
     </row>
     <row r="35" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="19" t="s">
+      <c r="A35" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="B35" s="19"/>
+      <c r="B35" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2626,8 +3174,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2664,7 +3212,7 @@
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="14">
         <v>3.19</v>
       </c>
       <c r="C4" s="18">
@@ -2676,7 +3224,7 @@
       <c r="F4" s="10">
         <v>5.3606106157362277</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="14">
         <f>B4*F4</f>
         <v>17.100347864198564</v>
       </c>
@@ -2685,7 +3233,7 @@
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="14">
         <v>2.59</v>
       </c>
       <c r="C5" s="18">
@@ -2697,7 +3245,7 @@
       <c r="F5" s="10">
         <v>2</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="14">
         <f t="shared" ref="G5:G11" si="0">B5*F5</f>
         <v>5.18</v>
       </c>
@@ -2706,7 +3254,7 @@
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="14">
         <v>2.29</v>
       </c>
       <c r="C6" s="18">
@@ -2718,7 +3266,7 @@
       <c r="F6" s="10">
         <v>2</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="14">
         <f t="shared" si="0"/>
         <v>4.58</v>
       </c>
@@ -2727,7 +3275,7 @@
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="14">
         <v>2.89</v>
       </c>
       <c r="C7" s="18">
@@ -2739,7 +3287,7 @@
       <c r="F7" s="10">
         <v>10</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="14">
         <f t="shared" si="0"/>
         <v>28.900000000000002</v>
       </c>
@@ -2748,7 +3296,7 @@
       <c r="A8" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="15">
         <v>1.89</v>
       </c>
       <c r="C8" s="18">
@@ -2761,7 +3309,7 @@
       <c r="F8" s="10">
         <v>10</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="15">
         <f t="shared" si="0"/>
         <v>18.899999999999999</v>
       </c>
@@ -2770,7 +3318,7 @@
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="14">
         <v>1.99</v>
       </c>
       <c r="C9" s="18">
@@ -2782,7 +3330,7 @@
       <c r="F9" s="10">
         <v>10</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="14">
         <f t="shared" si="0"/>
         <v>19.899999999999999</v>
       </c>
@@ -2791,7 +3339,7 @@
       <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="14">
         <v>1.99</v>
       </c>
       <c r="C10" s="18">
@@ -2803,7 +3351,7 @@
       <c r="F10" s="10">
         <v>9.3060553784107167</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="14">
         <f t="shared" si="0"/>
         <v>18.519050203037327</v>
       </c>
@@ -2812,7 +3360,7 @@
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="14">
         <v>2.4900000000000002</v>
       </c>
       <c r="C11" s="18">
@@ -2824,7 +3372,7 @@
       <c r="F11" s="10">
         <v>2</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="14">
         <f t="shared" si="0"/>
         <v>4.9800000000000004</v>
       </c>
@@ -2833,7 +3381,7 @@
       <c r="F12" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G12" s="16">
         <f>SUM(G4:G11)</f>
         <v>118.0593980672359</v>
       </c>
@@ -2843,15 +3391,15 @@
       <c r="G13" s="5"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="24" t="s">
+      <c r="C14" s="23" t="s">
         <v>30</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="23" t="s">
+      <c r="F14" s="22" t="s">
         <v>31</v>
       </c>
       <c r="G14" s="5"/>
@@ -2866,7 +3414,7 @@
       <c r="C15" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F15" s="21" t="s">
+      <c r="F15" s="20" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2941,7 +3489,8 @@
         <v>50000</v>
       </c>
       <c r="F20" s="4">
-        <v>50000</v>
+        <f>SUMPRODUCT(F25:F32,$F$4:$F$11)</f>
+        <v>50000.000355468423</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -3167,17 +3716,1134 @@
       </c>
     </row>
     <row r="35" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="19" t="s">
+      <c r="A35" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="B35" s="19"/>
+      <c r="B35" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A35:B35"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="10.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="14">
+        <v>3.19</v>
+      </c>
+      <c r="C4" s="18">
+        <v>2</v>
+      </c>
+      <c r="D4" s="18">
+        <v>10</v>
+      </c>
+      <c r="F4" s="10">
+        <v>6</v>
+      </c>
+      <c r="G4" s="14">
+        <f>B4*F4</f>
+        <v>19.14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="14">
+        <v>2.59</v>
+      </c>
+      <c r="C5" s="18">
+        <v>2</v>
+      </c>
+      <c r="D5" s="18">
+        <v>10</v>
+      </c>
+      <c r="F5" s="10">
+        <v>2</v>
+      </c>
+      <c r="G5" s="14">
+        <f t="shared" ref="G5:G11" si="0">B5*F5</f>
+        <v>5.18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="14">
+        <v>2.29</v>
+      </c>
+      <c r="C6" s="18">
+        <v>2</v>
+      </c>
+      <c r="D6" s="18">
+        <v>10</v>
+      </c>
+      <c r="F6" s="10">
+        <v>2</v>
+      </c>
+      <c r="G6" s="14">
+        <f t="shared" si="0"/>
+        <v>4.58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="14">
+        <v>2.89</v>
+      </c>
+      <c r="C7" s="18">
+        <v>2</v>
+      </c>
+      <c r="D7" s="18">
+        <v>10</v>
+      </c>
+      <c r="F7" s="10">
+        <v>10</v>
+      </c>
+      <c r="G7" s="14">
+        <f t="shared" si="0"/>
+        <v>28.900000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="15">
+        <v>1.89</v>
+      </c>
+      <c r="C8" s="18">
+        <v>2</v>
+      </c>
+      <c r="D8" s="18">
+        <v>10</v>
+      </c>
+      <c r="E8" s="9"/>
+      <c r="F8" s="10">
+        <v>10</v>
+      </c>
+      <c r="G8" s="15">
+        <f t="shared" si="0"/>
+        <v>18.899999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="14">
+        <v>1.99</v>
+      </c>
+      <c r="C9" s="18">
+        <v>2</v>
+      </c>
+      <c r="D9" s="18">
+        <v>10</v>
+      </c>
+      <c r="F9" s="10">
+        <v>10</v>
+      </c>
+      <c r="G9" s="14">
+        <f t="shared" si="0"/>
+        <v>19.899999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="14">
+        <v>1.99</v>
+      </c>
+      <c r="C10" s="18">
+        <v>2</v>
+      </c>
+      <c r="D10" s="18">
+        <v>10</v>
+      </c>
+      <c r="F10" s="10">
+        <v>10</v>
+      </c>
+      <c r="G10" s="14">
+        <f t="shared" si="0"/>
+        <v>19.899999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="14">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="C11" s="18">
+        <v>2</v>
+      </c>
+      <c r="D11" s="18">
+        <v>10</v>
+      </c>
+      <c r="F11" s="10">
+        <v>2</v>
+      </c>
+      <c r="G11" s="14">
+        <f t="shared" si="0"/>
+        <v>4.9800000000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F12" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="16">
+        <f>SUM(G4:G11)</f>
+        <v>121.48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14" s="5"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" s="20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16">
+        <v>700</v>
+      </c>
+      <c r="C16">
+        <v>20000</v>
+      </c>
+      <c r="F16" s="4">
+        <f>SUMPRODUCT(B25:B32,$F$4:$F$11)</f>
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17">
+        <v>700</v>
+      </c>
+      <c r="C17">
+        <v>20000</v>
+      </c>
+      <c r="F17" s="4">
+        <f>SUMPRODUCT(C25:C32,$F$4:$F$11)</f>
+        <v>1730</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18">
+        <v>700</v>
+      </c>
+      <c r="C18">
+        <v>20000</v>
+      </c>
+      <c r="F18" s="4">
+        <f>SUMPRODUCT(D25:D32,$F$4:$F$11)</f>
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19">
+        <v>700</v>
+      </c>
+      <c r="C19">
+        <v>20000</v>
+      </c>
+      <c r="F19" s="4">
+        <f>SUMPRODUCT(E25:E32,$F$4:$F$11)</f>
+        <v>720</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>50000</v>
+      </c>
+      <c r="F20" s="4">
+        <f>SUMPRODUCT(F25:F32,$F$4:$F$11)</f>
+        <v>51522</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21">
+        <v>16000</v>
+      </c>
+      <c r="C21">
+        <v>24000</v>
+      </c>
+      <c r="F21" s="4">
+        <f>SUMPRODUCT(G25:G32,$F$4:$F$11)</f>
+        <v>20240</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25">
+        <v>60</v>
+      </c>
+      <c r="C25">
+        <v>20</v>
+      </c>
+      <c r="D25">
+        <v>10</v>
+      </c>
+      <c r="E25">
+        <v>15</v>
+      </c>
+      <c r="F25">
+        <v>938</v>
+      </c>
+      <c r="G25">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26">
+        <v>8</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>20</v>
+      </c>
+      <c r="E26">
+        <v>20</v>
+      </c>
+      <c r="F26">
+        <v>2180</v>
+      </c>
+      <c r="G26">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27">
+        <v>8</v>
+      </c>
+      <c r="C27">
+        <v>10</v>
+      </c>
+      <c r="D27">
+        <v>15</v>
+      </c>
+      <c r="E27">
+        <v>10</v>
+      </c>
+      <c r="F27">
+        <v>945</v>
+      </c>
+      <c r="G27">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28">
+        <v>40</v>
+      </c>
+      <c r="C28">
+        <v>40</v>
+      </c>
+      <c r="D28">
+        <v>35</v>
+      </c>
+      <c r="E28">
+        <v>10</v>
+      </c>
+      <c r="F28">
+        <v>278</v>
+      </c>
+      <c r="G28">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" s="9">
+        <v>15</v>
+      </c>
+      <c r="C29" s="9">
+        <v>35</v>
+      </c>
+      <c r="D29" s="9">
+        <v>15</v>
+      </c>
+      <c r="E29" s="9">
+        <v>15</v>
+      </c>
+      <c r="F29" s="9">
+        <v>1182</v>
+      </c>
+      <c r="G29" s="9">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>2</v>
+      </c>
+      <c r="B30">
+        <v>70</v>
+      </c>
+      <c r="C30">
+        <v>30</v>
+      </c>
+      <c r="D30">
+        <v>15</v>
+      </c>
+      <c r="E30">
+        <v>15</v>
+      </c>
+      <c r="F30">
+        <v>896</v>
+      </c>
+      <c r="G30">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31">
+        <v>25</v>
+      </c>
+      <c r="C31">
+        <v>50</v>
+      </c>
+      <c r="D31">
+        <v>25</v>
+      </c>
+      <c r="E31">
+        <v>15</v>
+      </c>
+      <c r="F31">
+        <v>1329</v>
+      </c>
+      <c r="G31">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32">
+        <v>60</v>
+      </c>
+      <c r="C32">
+        <v>20</v>
+      </c>
+      <c r="D32">
+        <v>15</v>
+      </c>
+      <c r="E32">
+        <v>10</v>
+      </c>
+      <c r="F32">
+        <v>1397</v>
+      </c>
+      <c r="G32">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B35" s="26"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="10.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="14">
+        <v>3.19</v>
+      </c>
+      <c r="C4" s="18">
+        <v>2</v>
+      </c>
+      <c r="D4" s="18">
+        <v>10</v>
+      </c>
+      <c r="F4" s="10">
+        <v>9</v>
+      </c>
+      <c r="G4" s="14">
+        <f>B4*F4</f>
+        <v>28.71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="14">
+        <v>2.59</v>
+      </c>
+      <c r="C5" s="18">
+        <v>2</v>
+      </c>
+      <c r="D5" s="18">
+        <v>10</v>
+      </c>
+      <c r="F5" s="10">
+        <v>2</v>
+      </c>
+      <c r="G5" s="14">
+        <f t="shared" ref="G5:G11" si="0">B5*F5</f>
+        <v>5.18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="14">
+        <v>2.29</v>
+      </c>
+      <c r="C6" s="18">
+        <v>2</v>
+      </c>
+      <c r="D6" s="18">
+        <v>10</v>
+      </c>
+      <c r="F6" s="10">
+        <v>2</v>
+      </c>
+      <c r="G6" s="14">
+        <f t="shared" si="0"/>
+        <v>4.58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="14">
+        <v>2.89</v>
+      </c>
+      <c r="C7" s="18">
+        <v>2</v>
+      </c>
+      <c r="D7" s="18">
+        <v>10</v>
+      </c>
+      <c r="F7" s="10">
+        <v>8</v>
+      </c>
+      <c r="G7" s="14">
+        <f t="shared" si="0"/>
+        <v>23.12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="15">
+        <v>1.89</v>
+      </c>
+      <c r="C8" s="18">
+        <v>2</v>
+      </c>
+      <c r="D8" s="18">
+        <v>10</v>
+      </c>
+      <c r="E8" s="9"/>
+      <c r="F8" s="10">
+        <v>10</v>
+      </c>
+      <c r="G8" s="15">
+        <f t="shared" si="0"/>
+        <v>18.899999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="14">
+        <v>1.99</v>
+      </c>
+      <c r="C9" s="18">
+        <v>2</v>
+      </c>
+      <c r="D9" s="18">
+        <v>10</v>
+      </c>
+      <c r="F9" s="10">
+        <v>10</v>
+      </c>
+      <c r="G9" s="14">
+        <f t="shared" si="0"/>
+        <v>19.899999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="14">
+        <v>1.99</v>
+      </c>
+      <c r="C10" s="18">
+        <v>2</v>
+      </c>
+      <c r="D10" s="18">
+        <v>10</v>
+      </c>
+      <c r="F10" s="10">
+        <v>7</v>
+      </c>
+      <c r="G10" s="14">
+        <f t="shared" si="0"/>
+        <v>13.93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="14">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="C11" s="18">
+        <v>2</v>
+      </c>
+      <c r="D11" s="18">
+        <v>10</v>
+      </c>
+      <c r="F11" s="10">
+        <v>2</v>
+      </c>
+      <c r="G11" s="14">
+        <f t="shared" si="0"/>
+        <v>4.9800000000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F12" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="16">
+        <f>SUM(G4:G11)</f>
+        <v>119.30000000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14" s="5"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" s="20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16">
+        <v>700</v>
+      </c>
+      <c r="C16">
+        <v>20000</v>
+      </c>
+      <c r="F16" s="4">
+        <f>SUMPRODUCT(B25:B32,$F$4:$F$11)</f>
+        <v>2037</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17">
+        <v>700</v>
+      </c>
+      <c r="C17">
+        <v>20000</v>
+      </c>
+      <c r="F17" s="4">
+        <f>SUMPRODUCT(C25:C32,$F$4:$F$11)</f>
+        <v>1560</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18">
+        <v>700</v>
+      </c>
+      <c r="C18">
+        <v>20000</v>
+      </c>
+      <c r="F18" s="4">
+        <f>SUMPRODUCT(D25:D32,$F$4:$F$11)</f>
+        <v>945</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19">
+        <v>700</v>
+      </c>
+      <c r="C19">
+        <v>20000</v>
+      </c>
+      <c r="F19" s="4">
+        <f>SUMPRODUCT(E25:E32,$F$4:$F$11)</f>
+        <v>700</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>50000</v>
+      </c>
+      <c r="F20" s="4">
+        <f>SUMPRODUCT(F25:F32,$F$4:$F$11)</f>
+        <v>49793</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21">
+        <v>16000</v>
+      </c>
+      <c r="C21">
+        <v>24000</v>
+      </c>
+      <c r="F21" s="4">
+        <f>SUMPRODUCT(G25:G32,$F$4:$F$11)</f>
+        <v>19155</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25">
+        <v>60</v>
+      </c>
+      <c r="C25">
+        <v>20</v>
+      </c>
+      <c r="D25">
+        <v>10</v>
+      </c>
+      <c r="E25">
+        <v>15</v>
+      </c>
+      <c r="F25">
+        <v>938</v>
+      </c>
+      <c r="G25">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26">
+        <v>8</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>20</v>
+      </c>
+      <c r="E26">
+        <v>20</v>
+      </c>
+      <c r="F26">
+        <v>2180</v>
+      </c>
+      <c r="G26">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27">
+        <v>8</v>
+      </c>
+      <c r="C27">
+        <v>10</v>
+      </c>
+      <c r="D27">
+        <v>15</v>
+      </c>
+      <c r="E27">
+        <v>10</v>
+      </c>
+      <c r="F27">
+        <v>945</v>
+      </c>
+      <c r="G27">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28">
+        <v>40</v>
+      </c>
+      <c r="C28">
+        <v>40</v>
+      </c>
+      <c r="D28">
+        <v>35</v>
+      </c>
+      <c r="E28">
+        <v>10</v>
+      </c>
+      <c r="F28">
+        <v>278</v>
+      </c>
+      <c r="G28">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" s="9">
+        <v>15</v>
+      </c>
+      <c r="C29" s="9">
+        <v>35</v>
+      </c>
+      <c r="D29" s="9">
+        <v>15</v>
+      </c>
+      <c r="E29" s="9">
+        <v>15</v>
+      </c>
+      <c r="F29" s="9">
+        <v>1182</v>
+      </c>
+      <c r="G29" s="9">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>2</v>
+      </c>
+      <c r="B30">
+        <v>70</v>
+      </c>
+      <c r="C30">
+        <v>30</v>
+      </c>
+      <c r="D30">
+        <v>15</v>
+      </c>
+      <c r="E30">
+        <v>15</v>
+      </c>
+      <c r="F30">
+        <v>896</v>
+      </c>
+      <c r="G30">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31">
+        <v>25</v>
+      </c>
+      <c r="C31">
+        <v>50</v>
+      </c>
+      <c r="D31">
+        <v>25</v>
+      </c>
+      <c r="E31">
+        <v>15</v>
+      </c>
+      <c r="F31">
+        <v>1329</v>
+      </c>
+      <c r="G31">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32">
+        <v>60</v>
+      </c>
+      <c r="C32">
+        <v>20</v>
+      </c>
+      <c r="D32">
+        <v>15</v>
+      </c>
+      <c r="E32">
+        <v>10</v>
+      </c>
+      <c r="F32">
+        <v>1397</v>
+      </c>
+      <c r="G32">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B35" s="26"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3307,12 +4973,80 @@
 display solve_result &gt; Sheet;</FileText>
       <ParentWorksheetName>diet2b</ParentWorksheetName>
     </StoredFile>
+    <StoredFile>
+      <FileName>Untitled</FileName>
+      <LanguageName>AMPL</LanguageName>
+      <ModelPaneVisible>true</ModelPaneVisible>
+      <ModelSettings/>
+      <FileText>set NUTR;               #define the index A,C,B1,B2
+set FOOD;               #define the index BEEF,...TUR
+param cost {FOOD} &gt; 0;   #cost of FOOD items with fixed lower limit
+param f_min {FOOD} &gt;= 0;
+param f_max {j in FOOD} &gt;= f_min[j];
+param n_min {NUTR} &gt;= 0;
+param n_max {i in NUTR} &gt;= n_min[i];
+param amt {NUTR,FOOD} &gt;= 0;
+# Decision Variables to solve for
+var Buy {j in FOOD} &gt;= f_min[j], &lt;= f_max[j];
+minimize Total_Cost:  sum {j in FOOD} cost[j] * Buy[j];
+subject to Diet {i in NUTR}:
+   n_min[i] &lt;= sum {j in FOOD} amt[i,j] * Buy[j] &lt;= n_max[i];
+#===================================================================
+# All lines below are optional if FixMinorErrors is checked
+#===================================================================
+# Get the data from the sheet for the sets and params defined above
+data SheetData.dat;
+# Solve the problem
+option solver IPOPT;    #Interior Point Optimization 
+#option solver cbc;
+solve;
+#AFTER THE SOLUTION rounded to near integer to see Sodium violation.
+let Buy["BEEF"] := 6;
+let Buy["SPG"]  := 10;
+display Buy &gt; Sheet;
+display solve_result &gt; Sheet;
+</FileText>
+      <ParentWorksheetName>diet2aForceInt</ParentWorksheetName>
+    </StoredFile>
+    <StoredFile>
+      <FileName>Untitled</FileName>
+      <LanguageName>AMPL</LanguageName>
+      <ModelPaneVisible>true</ModelPaneVisible>
+      <ModelSettings/>
+      <FileText>set NUTR;               #define the index A,C,B1,B2
+set FOOD;               #define the index BEEF,...TUR
+param cost {FOOD} &gt; 0;   #cost of FOOD items with fixed lower limit
+param f_min {FOOD} &gt;= 0;
+param f_max {j in FOOD} &gt;= f_min[j];
+param n_min {NUTR} &gt;= 0;
+param n_max {i in NUTR} &gt;= n_min[i];
+param amt {NUTR,FOOD} &gt;= 0;
+# Decision Variables to solve for
+# WITH INTEGRALITY RESTRICTION
+var Buy {j in FOOD} integer &gt;= f_min[j], &lt;= f_max[j];
+minimize Total_Cost:  sum {j in FOOD} cost[j] * Buy[j];
+subject to Diet {i in NUTR}:
+   n_min[i] &lt;= sum {j in FOOD} amt[i,j] * Buy[j] &lt;= n_max[i];
+#===================================================================
+# All lines below are optional if FixMinorErrors is checked
+#===================================================================
+# Get the data from the sheet for the sets and params defined above
+data SheetData.dat;
+# Solve the problem
+#option solver IPOPT;    #Interior Point Optimization 
+option solver cbc;       #switch to COIN-CMDC solver
+solve;
+display Buy &gt; Sheet;
+display solve_result &gt; Sheet;
+</FileText>
+      <ParentWorksheetName>diet2aIntRestrict</ParentWorksheetName>
+    </StoredFile>
   </StoredFiles>
 </StoredFilesList>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{30EA6AF1-73FB-440E-B36A-4278AC8067E3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F55930B5-DAE4-486C-83C2-6922556B73B0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://opensolver.org"/>

</xml_diff>